<commit_message>
New instances and RO
</commit_message>
<xml_diff>
--- a/input_small.xlsx
+++ b/input_small.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/UC/PhD/Math models/Robust/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/UC/PhD/Math models/Electric Bus Smart Charging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587EB6F-0EA8-C049-8349-CCC99C342440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D91D5E-141D-6541-83A3-1B0B8CCD9820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
+    <workbookView xWindow="-31520" yWindow="2060" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{933CD496-2CE3-3447-B44F-7F4C3643C8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Buses" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -169,7 +169,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D4C7943-5FF2-FD4F-90F7-B7009FED3143}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +713,7 @@
       <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2">
         <f>12/60</f>
         <v>0.2</v>
       </c>
@@ -801,7 +800,7 @@
   <dimension ref="A1:C1441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13792,10 +13791,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E9005A-C93F-D246-A03F-07B7DAAF214E}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13862,111 +13861,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f>$A$2*3</f>
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>6.5087999999999999</v>
-      </c>
-      <c r="C4">
-        <v>240</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f>$A$2*4</f>
-        <v>5.333333333333333</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>8.6783999999999999</v>
-      </c>
-      <c r="C5">
-        <v>320</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f>$A$2*5</f>
-        <v>6.6666666666666661</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>10.847999999999999</v>
-      </c>
-      <c r="C6">
-        <v>400</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <f>$A$2*6</f>
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>13.0176</v>
-      </c>
-      <c r="C7">
-        <v>480</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <f>$A$2*7</f>
-        <v>9.3333333333333321</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>15.187200000000001</v>
-      </c>
-      <c r="C8">
-        <v>560</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <f>$A$2*8</f>
-        <v>10.666666666666666</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>17.3568</v>
-      </c>
-      <c r="C9">
-        <v>640</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>